<commit_message>
update email reporter listenter
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/prepareStatement/sql_ps_dml_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/prepareStatement/sql_ps_dml_cases.xlsx
@@ -548,8 +548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
add case of preparedStatement about set values for insert multiple record sql
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/prepareStatement/sql_ps_dml_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/prepareStatement/sql_ps_dml_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
   <si>
     <t>TestID</t>
   </si>
@@ -149,10 +149,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>插入语句中使用prepareStatement</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>insert into $schema17 values(?,?,?,?,?,?,?,?,?,?,?,?)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -172,7 +168,37 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>ps_dml_004</t>
+  </si>
+  <si>
+    <t>插入单条语句中使用prepareStatement</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>插入多条语句中使用prepareStatement</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into $schema17 values(?,?,?,?,?,?,?,?,?,?,?,?),(?,?,?,?,?,?,?,?,?,?,?,?),(?,?,?,?,?,?,?,?,?,?,?,?)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>1001,JDK_Home,33,35890926187,456.99,98472345827.1299,Tust Plaza 01,19891203,162530,20230320183000,100812,false</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/prepareStatement/expectedresult/ps_dml_004.csv</t>
+  </si>
+  <si>
+    <t>1001,JDK_Home,33,35890926187,456.99,98472345827.1299,Tust Plaza 01,19891203,162530,20230320183000,100812,false,1002,zhangsan,-18,88,2.5,12.3,shanghai,20150910,034510,20011111180507,110586,true,1003,awJDs,1,-127,1000.0,-1453.9999,pingYang1,19611001,190000,20101001020202,210092,true</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Integer,Varchar,Integer,Bigint,Float,Double,Varchar,Date,Time,Timestamp,Varchar,Boolean,Integer,Varchar,Integer,Bigint,Float,Double,Varchar,Date,Time,Timestamp,Varchar,Boolean,Integer,Varchar,Integer,Bigint,Float,Double,Varchar,Date,Time,Timestamp,Varchar,Boolean</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -546,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -706,7 +732,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>10</v>
@@ -715,24 +741,62 @@
         <v>11</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4" s="2" t="s">
+      <c r="L4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A5" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="N4" s="5" t="s">
+      <c r="M5" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>